<commit_message>
update to version 2.22.0-SNAPSHOT
</commit_message>
<xml_diff>
--- a/cs-models/eai/cms/nga.gov/search.xlsx
+++ b/cs-models/eai/cms/nga.gov/search.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aradeva\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="12435"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>cultObj:title</t>
   </si>
@@ -61,6 +66,24 @@
   </si>
   <si>
     <t>nga:artistNames</t>
+  </si>
+  <si>
+    <t>between</t>
+  </si>
+  <si>
+    <t>cultObj:lastModified</t>
+  </si>
+  <si>
+    <t>emf:modifiedOn</t>
+  </si>
+  <si>
+    <t>(system)API Search Form Visibility </t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -374,7 +397,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -382,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D5"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,7 +418,7 @@
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -408,8 +431,11 @@
       <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -422,8 +448,11 @@
       <c r="D2">
         <v>1</v>
       </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -436,8 +465,11 @@
       <c r="D3">
         <v>2</v>
       </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -450,8 +482,11 @@
       <c r="D4">
         <v>3</v>
       </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -463,9 +498,27 @@
       </c>
       <c r="D5">
         <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>